<commit_message>
Added more test case, application submission
</commit_message>
<xml_diff>
--- a/tests/testplan/North West Recruitment Portal – QA Test Plan.xlsx
+++ b/tests/testplan/North West Recruitment Portal – QA Test Plan.xlsx
@@ -1,19 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rukmal/Projects/demo_selenium_javascripts/tests/testplan/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31505F05-8CAC-D747-8F0B-4E684B47C22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Test Plan" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Test Case Admin Login" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Test Case Add Vacancy" sheetId="3" r:id="rId6"/>
+    <sheet name="Test Plan" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Case Admin Login" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Case Add Vacancy" sheetId="3" r:id="rId3"/>
+    <sheet name="Candidate Submits application" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="197">
   <si>
     <t>North West Recruitment Portal – QA Test Plan</t>
   </si>
@@ -539,34 +550,114 @@
     <t>Verify Successfully Save Message
 Verify it displays in the Vacancy Dashboard</t>
   </si>
+  <si>
+    <t>TC-APP-001</t>
+  </si>
+  <si>
+    <t>Candidate can submit a job application (happy path)</t>
+  </si>
+  <si>
+    <t>Verify a candidate can successfully submit an application for a listed vacancy, including CV upload and consent.</t>
+  </si>
+  <si>
+    <t>Functional, Usability, Security (Confidentiality)</t>
+  </si>
+  <si>
+    <t>At least one active vacancy is visible on the public site</t>
+  </si>
+  <si>
+    <t>The application form is reachable from the vacancy detail page (e.g., Apply button).</t>
+  </si>
+  <si>
+    <t>Test file available: valid_cv.pdf (PDF, &lt; 10MB).</t>
+  </si>
+  <si>
+    <t>Browser has no active session; cookies enabled; JavaScript enabled.</t>
+  </si>
+  <si>
+    <t>Navigate to public job listings page</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Listings load; at least one vacancy visible.</t>
+  </si>
+  <si>
+    <t>Select an Vacancy</t>
+  </si>
+  <si>
+    <t>Company: mSupply</t>
+  </si>
+  <si>
+    <t>Vacancy detail shows role title, description, and Apply button</t>
+  </si>
+  <si>
+    <t>Click Apply</t>
+  </si>
+  <si>
+    <t>Application form is displayed (Vacancy Details, name, email, phone, CV upload, consent, submit).
+Verify Company Name:
+Verify Vacancy Details
+Verify candidates personal information section is visible</t>
+  </si>
+  <si>
+    <t>Scroll to jobs</t>
+  </si>
+  <si>
+    <t>Display web page elements top to down</t>
+  </si>
+  <si>
+    <t>Click Sort by Office link</t>
+  </si>
+  <si>
+    <t>Sorting option brings the necessary vacancies to the window</t>
+  </si>
+  <si>
+    <t>Applicant Details, and pdf files</t>
+  </si>
+  <si>
+    <t>Click Submit button</t>
+  </si>
+  <si>
+    <t>Verify Successfully "Thank you for your application"</t>
+  </si>
+  <si>
+    <t>Network is online (upload uses a third-party service like Cloudinary).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="24.0"/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -575,7 +666,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -597,7 +688,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -611,70 +708,59 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -864,523 +950,531 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:E82"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="19.0"/>
-    <col customWidth="1" min="2" max="2" width="28.25"/>
-    <col customWidth="1" min="3" max="3" width="48.13"/>
-    <col customWidth="1" min="4" max="4" width="38.13"/>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="28.1640625" customWidth="1"/>
+    <col min="3" max="3" width="48.1640625" customWidth="1"/>
+    <col min="4" max="4" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4" t="s">
+      <c r="C5" s="11"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="2" t="s">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15">
-      <c r="B15" s="5" t="s">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16">
-      <c r="B16" s="6" t="s">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17">
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18">
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20">
-      <c r="B20" s="6" t="s">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21">
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27">
-      <c r="B27" s="6" t="s">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28">
-      <c r="B28" s="6" t="s">
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29">
-      <c r="B29" s="6" t="s">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30">
-      <c r="B30" s="6" t="s">
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31">
-      <c r="B31" s="6" t="s">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35">
-      <c r="B35" s="2" t="s">
+    <row r="35" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36">
-      <c r="B36" s="5" t="s">
+    <row r="36" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B36" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="37">
-      <c r="B37" s="6" t="s">
+    <row r="37" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38">
-      <c r="B38" s="6" t="s">
+    <row r="38" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39">
-      <c r="B39" s="6" t="s">
+    <row r="39" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41">
-      <c r="B41" s="2" t="s">
+    <row r="41" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B41" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42">
-      <c r="B42" s="5" t="s">
+    <row r="42" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="43">
-      <c r="B43" s="6" t="s">
+    <row r="43" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B43" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44">
-      <c r="B44" s="6" t="s">
+    <row r="44" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="45">
-      <c r="B45" s="6" t="s">
+    <row r="45" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="47">
-      <c r="B47" s="2" t="s">
+    <row r="47" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B47" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="48">
-      <c r="B48" s="5" t="s">
+    <row r="48" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B48" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="49">
-      <c r="B49" s="6" t="s">
+    <row r="49" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B49" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="6" t="s">
+      <c r="C49" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="50">
-      <c r="B50" s="6" t="s">
+    <row r="50" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B50" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="51">
-      <c r="B51" s="6" t="s">
+    <row r="51" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B51" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="52">
-      <c r="B52" s="6" t="s">
+    <row r="52" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B52" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" s="2" t="s">
+    <row r="54" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="55">
-      <c r="B55" s="2" t="s">
+    <row r="55" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B55" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="56">
-      <c r="B56" s="5" t="s">
+    <row r="56" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B56" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57">
-      <c r="B57" s="6" t="s">
+    <row r="57" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B57" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="58">
-      <c r="B58" s="6" t="s">
+    <row r="58" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B58" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59">
-      <c r="B59" s="6" t="s">
+    <row r="59" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B59" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60">
-      <c r="B60" s="6" t="s">
+    <row r="60" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B60" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="62">
-      <c r="B62" s="2" t="s">
+    <row r="62" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B62" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="63">
-      <c r="B63" s="5" t="s">
+    <row r="63" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B63" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="64">
-      <c r="B64" s="6" t="s">
+    <row r="64" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B64" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="65">
-      <c r="B65" s="6" t="s">
+    <row r="65" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B65" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="66">
-      <c r="B66" s="6" t="s">
+    <row r="66" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B66" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="67">
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-    </row>
-    <row r="68">
-      <c r="B68" s="2" t="s">
+    <row r="67" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+    </row>
+    <row r="68" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B68" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="69">
-      <c r="B69" s="5" t="s">
+    <row r="69" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B69" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C69" s="5" t="s">
+      <c r="C69" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70">
-      <c r="B70" s="6" t="s">
+    <row r="70" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B70" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="71">
-      <c r="B71" s="6" t="s">
+    <row r="71" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B71" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="72">
-      <c r="B72" s="6" t="s">
+    <row r="72" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B72" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="73">
-      <c r="B73" s="6" t="s">
+    <row r="73" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B73" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" s="2" t="s">
+    <row r="76" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="A76" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="77">
-      <c r="B77" s="5" t="s">
+    <row r="77" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B77" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C77" s="5" t="s">
+      <c r="C77" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="78">
-      <c r="B78" s="6" t="s">
+    <row r="78" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B78" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C78" s="6" t="s">
+      <c r="C78" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79">
-      <c r="B79" s="6" t="s">
+    <row r="79" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B79" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C79" s="6" t="s">
+      <c r="C79" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="80">
-      <c r="B80" s="6" t="s">
+    <row r="80" spans="1:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B80" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C80" s="6" t="s">
+      <c r="C80" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="81">
-      <c r="B81" s="6" t="s">
+    <row r="81" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B81" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="82">
-      <c r="B82" s="6" t="s">
+    <row r="82" spans="2:3" ht="13" x14ac:dyDescent="0.15">
+      <c r="B82" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C82" s="4" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1389,666 +1483,939 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B5:C5"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="79.13"/>
-    <col customWidth="1" min="4" max="4" width="17.13"/>
-    <col customWidth="1" min="5" max="5" width="40.13"/>
+    <col min="3" max="3" width="79.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5">
-      <c r="B5" s="6" t="s">
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6">
-      <c r="B6" s="6" t="s">
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7">
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="8">
-      <c r="B8" s="6" t="s">
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="8" t="s">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="C13" s="9" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="C14" s="9" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="C15" s="9" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="5">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="C16" s="9" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="5">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="7">
-        <v>5.0</v>
-      </c>
-      <c r="C17" s="9" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="5">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="5" t="s">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21">
-      <c r="B21" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="C21" s="6" t="s">
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="22">
-      <c r="B22" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="C22" s="6" t="s">
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="23">
-      <c r="B23" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="C23" s="6" t="s">
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="5">
+        <v>3</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="24">
-      <c r="B24" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="C24" s="6" t="s">
+    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="5">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="25">
-      <c r="B25" s="7">
-        <v>5.0</v>
-      </c>
-      <c r="C25" s="6" t="s">
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="26">
-      <c r="B26" s="7">
-        <v>6.0</v>
-      </c>
-      <c r="C26" s="6" t="s">
+    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="5">
+        <v>6</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="27">
-      <c r="B27" s="7">
-        <v>7.0</v>
-      </c>
-      <c r="C27" s="6" t="s">
+    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="5">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28">
-      <c r="B28" s="7">
-        <v>8.0</v>
-      </c>
-      <c r="C28" s="6" t="s">
+    <row r="28" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="5">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E28" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="29">
-      <c r="B29" s="7">
-        <v>9.0</v>
-      </c>
-      <c r="C29" s="10" t="s">
+    <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="5">
+        <v>9</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="4" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="30">
-      <c r="B30" s="7">
-        <v>10.0</v>
-      </c>
-      <c r="C30" s="10" t="s">
+    <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="5">
+        <v>10</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E30" s="4" t="s">
         <v>151</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:E34"/>
+  <sheetViews>
+    <sheetView zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="79.1640625" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="48.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="5">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="5">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="5">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="5">
+        <v>3</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="5">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="5">
+        <v>6</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="5">
+        <v>7</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="5">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="5">
+        <v>9</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B30" s="5">
+        <v>10</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B31" s="5">
+        <v>11</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="5">
+        <v>12</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="5"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B34" s="5"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB023A53-DAB0-6647-95C8-5F4A79EFEE83}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="B2:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="79.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="48.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+    </row>
+    <row r="14" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B15" s="5">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="5">
+        <v>4</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="5">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B23" s="5">
+        <v>3</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B24" s="5">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="70" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="5">
+        <v>5</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="5">
+        <v>6</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD0AE22-2D3C-E044-8C7F-AAA10DCEFEB4}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="3" max="3" width="79.13"/>
-    <col customWidth="1" min="4" max="4" width="17.13"/>
-    <col customWidth="1" min="5" max="5" width="40.13"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="B2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13">
-      <c r="B13" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14">
-      <c r="B14" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15">
-      <c r="B15" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16">
-      <c r="B16" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17">
-      <c r="B17" s="7">
-        <v>5.0</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20">
-      <c r="B20" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" s="7">
-        <v>3.0</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" s="7">
-        <v>4.0</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" s="7">
-        <v>5.0</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" s="7">
-        <v>6.0</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" s="7">
-        <v>7.0</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28">
-      <c r="B28" s="7">
-        <v>8.0</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="7">
-        <v>9.0</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" s="7">
-        <v>10.0</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" s="7">
-        <v>11.0</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" s="7">
-        <v>12.0</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" s="7"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34">
-      <c r="B34" s="7"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>